<commit_message>
correction type filler bug ano mco 18
</commit_message>
<xml_diff>
--- a/formats/excel/Formats RSA ANO 18.xlsx
+++ b/formats/excel/Formats RSA ANO 18.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267">
   <si>
     <t>libelle</t>
   </si>
@@ -641,9 +641,6 @@
   </si>
   <si>
     <t>Filler</t>
-  </si>
-  <si>
-    <t>C</t>
   </si>
   <si>
     <t xml:space="preserve">Rang de naissance </t>
@@ -829,9 +826,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -877,9 +874,39 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -892,39 +919,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -954,20 +958,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -977,9 +967,32 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -992,30 +1005,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1042,13 +1039,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1060,13 +1057,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1078,13 +1093,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1096,13 +1105,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1120,37 +1123,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1162,67 +1213,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1277,26 +1274,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1351,6 +1348,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1359,165 +1371,150 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1890,9 +1887,9 @@
   <dimension ref="A1:F131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63:B74"/>
+      <selection pane="bottomLeft" activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="5"/>
@@ -4104,7 +4101,7 @@
         <v>207</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="D101" s="6">
         <v>3</v>
@@ -4120,10 +4117,10 @@
     </row>
     <row r="102" ht="15" spans="1:6">
       <c r="A102" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="B102" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>8</v>
@@ -4142,10 +4139,10 @@
     </row>
     <row r="103" ht="15" spans="1:6">
       <c r="A103" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B103" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>212</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>8</v>
@@ -4164,10 +4161,10 @@
     </row>
     <row r="104" ht="15" spans="1:6">
       <c r="A104" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B104" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>214</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>8</v>
@@ -4186,10 +4183,10 @@
     </row>
     <row r="105" ht="15" spans="1:6">
       <c r="A105" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B105" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>216</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>8</v>
@@ -4208,10 +4205,10 @@
     </row>
     <row r="106" ht="15" spans="1:6">
       <c r="A106" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B106" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>218</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>8</v>
@@ -4230,10 +4227,10 @@
     </row>
     <row r="107" ht="15" spans="1:6">
       <c r="A107" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B107" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>220</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>8</v>
@@ -4252,10 +4249,10 @@
     </row>
     <row r="108" ht="15" spans="1:6">
       <c r="A108" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B108" s="3" t="s">
         <v>221</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>222</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>8</v>
@@ -4274,10 +4271,10 @@
     </row>
     <row r="109" spans="1:6">
       <c r="A109" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="B109" s="3" t="s">
         <v>223</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>224</v>
       </c>
       <c r="C109" t="s">
         <v>8</v>
@@ -4296,10 +4293,10 @@
     </row>
     <row r="110" spans="1:6">
       <c r="A110" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="B110" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="B110" s="3" t="s">
-        <v>226</v>
       </c>
       <c r="C110" t="s">
         <v>8</v>
@@ -4318,10 +4315,10 @@
     </row>
     <row r="111" spans="1:6">
       <c r="A111" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="B111" s="3" t="s">
         <v>227</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>228</v>
       </c>
       <c r="C111" t="s">
         <v>8</v>
@@ -4340,10 +4337,10 @@
     </row>
     <row r="112" spans="1:6">
       <c r="A112" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="B112" s="3" t="s">
         <v>229</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>230</v>
       </c>
       <c r="C112" t="s">
         <v>8</v>
@@ -4362,10 +4359,10 @@
     </row>
     <row r="113" spans="1:6">
       <c r="A113" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="B113" s="3" t="s">
         <v>231</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="C113" t="s">
         <v>8</v>
@@ -4384,10 +4381,10 @@
     </row>
     <row r="114" spans="1:6">
       <c r="A114" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="B114" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>234</v>
       </c>
       <c r="C114" t="s">
         <v>8</v>
@@ -4406,10 +4403,10 @@
     </row>
     <row r="115" spans="1:6">
       <c r="A115" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="B115" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>236</v>
       </c>
       <c r="C115" t="s">
         <v>8</v>
@@ -4428,10 +4425,10 @@
     </row>
     <row r="116" spans="1:6">
       <c r="A116" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="B116" s="3" t="s">
         <v>237</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>238</v>
       </c>
       <c r="C116" t="s">
         <v>8</v>
@@ -4450,10 +4447,10 @@
     </row>
     <row r="117" ht="15" spans="1:6">
       <c r="A117" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="B117" s="15" t="s">
         <v>239</v>
-      </c>
-      <c r="B117" s="15" t="s">
-        <v>240</v>
       </c>
       <c r="C117" t="s">
         <v>176</v>
@@ -4472,10 +4469,10 @@
     </row>
     <row r="118" ht="15" spans="1:6">
       <c r="A118" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B118" s="15" t="s">
         <v>241</v>
-      </c>
-      <c r="B118" s="15" t="s">
-        <v>242</v>
       </c>
       <c r="C118" t="s">
         <v>8</v>
@@ -4494,10 +4491,10 @@
     </row>
     <row r="119" ht="15" spans="1:6">
       <c r="A119" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="B119" s="15" t="s">
         <v>243</v>
-      </c>
-      <c r="B119" s="15" t="s">
-        <v>244</v>
       </c>
       <c r="C119" t="s">
         <v>8</v>
@@ -4516,10 +4513,10 @@
     </row>
     <row r="120" ht="15" spans="1:6">
       <c r="A120" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="B120" s="15" t="s">
         <v>245</v>
-      </c>
-      <c r="B120" s="15" t="s">
-        <v>246</v>
       </c>
       <c r="C120" t="s">
         <v>8</v>
@@ -4538,10 +4535,10 @@
     </row>
     <row r="121" ht="15" spans="1:6">
       <c r="A121" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="B121" s="15" t="s">
         <v>247</v>
-      </c>
-      <c r="B121" s="15" t="s">
-        <v>248</v>
       </c>
       <c r="C121" t="s">
         <v>8</v>
@@ -4560,10 +4557,10 @@
     </row>
     <row r="122" ht="15" spans="1:6">
       <c r="A122" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="B122" s="15" t="s">
         <v>249</v>
-      </c>
-      <c r="B122" s="15" t="s">
-        <v>250</v>
       </c>
       <c r="C122" t="s">
         <v>8</v>
@@ -4582,10 +4579,10 @@
     </row>
     <row r="123" ht="15" spans="1:6">
       <c r="A123" s="20" t="s">
+        <v>250</v>
+      </c>
+      <c r="B123" s="15" t="s">
         <v>251</v>
-      </c>
-      <c r="B123" s="15" t="s">
-        <v>252</v>
       </c>
       <c r="C123" t="s">
         <v>8</v>
@@ -4604,10 +4601,10 @@
     </row>
     <row r="124" ht="15" spans="1:6">
       <c r="A124" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="B124" s="15" t="s">
         <v>253</v>
-      </c>
-      <c r="B124" s="15" t="s">
-        <v>254</v>
       </c>
       <c r="C124" t="s">
         <v>8</v>
@@ -4626,10 +4623,10 @@
     </row>
     <row r="125" ht="15" spans="1:6">
       <c r="A125" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="B125" s="15" t="s">
         <v>255</v>
-      </c>
-      <c r="B125" s="15" t="s">
-        <v>256</v>
       </c>
       <c r="C125" t="s">
         <v>8</v>
@@ -4648,10 +4645,10 @@
     </row>
     <row r="126" ht="15" spans="1:6">
       <c r="A126" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="B126" s="15" t="s">
         <v>257</v>
-      </c>
-      <c r="B126" s="15" t="s">
-        <v>258</v>
       </c>
       <c r="C126" t="s">
         <v>8</v>
@@ -4670,10 +4667,10 @@
     </row>
     <row r="127" ht="15" spans="1:6">
       <c r="A127" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="B127" s="15" t="s">
         <v>259</v>
-      </c>
-      <c r="B127" s="15" t="s">
-        <v>260</v>
       </c>
       <c r="C127" t="s">
         <v>8</v>
@@ -4692,10 +4689,10 @@
     </row>
     <row r="128" ht="15" spans="1:6">
       <c r="A128" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="B128" s="15" t="s">
         <v>261</v>
-      </c>
-      <c r="B128" s="15" t="s">
-        <v>262</v>
       </c>
       <c r="C128" t="s">
         <v>8</v>
@@ -4715,7 +4712,7 @@
     <row r="129" spans="1:6">
       <c r="A129" s="17"/>
       <c r="B129" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C129" t="s">
         <v>8</v>
@@ -4734,10 +4731,10 @@
     </row>
     <row r="130" spans="1:6">
       <c r="A130" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="B130" s="3" t="s">
         <v>264</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>265</v>
       </c>
       <c r="C130" t="s">
         <v>8</v>
@@ -4756,10 +4753,10 @@
     </row>
     <row r="131" spans="1:6">
       <c r="A131" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="B131" s="3" t="s">
         <v>266</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>267</v>
       </c>
       <c r="C131" t="s">
         <v>8</v>

</xml_diff>